<commit_message>
Added a new tab for CAVV with a graph that shows age category per SAFEKits and added new data for Dept. Correccion y Rehabilitacion
</commit_message>
<xml_diff>
--- a/data/Prevencion_de_violencia_de_genero_CAVV/SAFEkits.xlsx
+++ b/data/Prevencion_de_violencia_de_genero_CAVV/SAFEkits.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28512"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix.baez\Documents\ViolenciaGeneroPR\data\Prevencion_de_violencia_de_genero_CAVV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlando.hernandez\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67720C20-F01A-4676-AF5B-0B84DBA9E995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" xr2:uid="{A7F466B2-A1CC-45B7-9CA9-433210358014}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Edades" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="24">
   <si>
     <t>Equipo de recolección de evidencia en casos de violencia sexual (RAPE kits/ SAFE Kits)</t>
   </si>
@@ -101,12 +101,21 @@
   <si>
     <t>TOTAL:</t>
   </si>
+  <si>
+    <t>Cantidad de menores</t>
+  </si>
+  <si>
+    <t>Cantidad de mayores</t>
+  </si>
+  <si>
+    <t>No identificado</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,33 +165,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -219,7 +203,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="51">
+  <borders count="61">
     <border>
       <left/>
       <right/>
@@ -887,11 +871,145 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -938,51 +1056,202 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -990,177 +1259,59 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1181,7 +1332,6 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1216,7 +1366,6 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1235,13 +1384,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thick">
-          <color rgb="FF000000"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1268,10 +1410,16 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thick">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1287,7 +1435,6 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1320,7 +1467,6 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1340,18 +1486,18 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thick">
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
+      <border>
+        <bottom style="thick">
           <color rgb="FF000000"/>
         </bottom>
       </border>
@@ -1370,22 +1516,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{92DDFBE8-06E8-4CE8-BB4B-5ECAA7FA103A}" name="Table1" displayName="Table1" ref="A30:B36" totalsRowShown="0" headerRowBorderDxfId="7" tableBorderDxfId="8">
-  <autoFilter ref="A30:B36" xr:uid="{92DDFBE8-06E8-4CE8-BB4B-5ECAA7FA103A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A42:B48" totalsRowShown="0" headerRowBorderDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="A42:B48"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{92659182-5D6E-4B7A-9FC7-AE412E6B5424}" name="Año" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{A0598327-45C3-463B-A293-2E67475C25E3}" name="Total con querella" dataDxfId="5"/>
+    <tableColumn id="1" name="Año" dataDxfId="6"/>
+    <tableColumn id="2" name="Total con querella" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0760F218-ED3B-4D73-A041-C1374446853C}" name="Table2" displayName="Table2" ref="I30:J37" totalsRowShown="0" dataDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3">
-  <autoFilter ref="I30:J37" xr:uid="{0760F218-ED3B-4D73-A041-C1374446853C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="I42:J49" totalsRowShown="0" dataDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="2">
+  <autoFilter ref="I42:J49"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{5E0D2130-1DAD-4A76-87FC-6840A9D08990}" name="Año" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{794EF59B-6C25-450C-BE17-11F49C04336E}" name="Total sin querella" dataDxfId="0"/>
+    <tableColumn id="1" name="Año" dataDxfId="1"/>
+    <tableColumn id="2" name="Total sin querella" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1707,59 +1853,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DE5160-F1D0-4B5C-AC51-73AF13242354}">
-  <dimension ref="A1:M37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.375" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
+    <col min="4" max="4" width="14.75" customWidth="1"/>
+    <col min="5" max="5" width="12.625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.75">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:13" ht="18">
+      <c r="A1" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-    </row>
-    <row r="3" spans="1:13" ht="21">
-      <c r="A3" s="17" t="s">
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+    </row>
+    <row r="3" spans="1:13" ht="20.25">
+      <c r="A3" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="I3" s="17" t="s">
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="I3" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-    </row>
-    <row r="4" spans="1:13" ht="30">
-      <c r="A4" s="42" t="s">
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+    </row>
+    <row r="4" spans="1:13" ht="30.75" thickBot="1">
+      <c r="A4" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1774,7 +1920,7 @@
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="48" t="s">
+      <c r="I4" s="27" t="s">
         <v>3</v>
       </c>
       <c r="J4" s="13" t="s">
@@ -1790,368 +1936,368 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="36">
-        <v>2021</v>
+    <row r="5" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A5" s="97">
+        <v>2019</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="67">
-        <v>15</v>
-      </c>
-      <c r="I5" s="43">
-        <v>2021</v>
+      <c r="E5" s="3">
+        <v>14</v>
+      </c>
+      <c r="I5" s="100">
+        <v>2019</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="K5" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="56">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="37"/>
+      <c r="M5" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15" customHeight="1">
+      <c r="A6" s="98"/>
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="7">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="68">
+      <c r="E6" s="7">
         <v>13</v>
       </c>
-      <c r="I6" s="44"/>
+      <c r="I6" s="101"/>
       <c r="J6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="K6" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="57">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="37"/>
+      <c r="M6" s="72">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15" customHeight="1">
+      <c r="A7" s="98"/>
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="5">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="69">
-        <v>7</v>
-      </c>
-      <c r="I7" s="44"/>
+      <c r="E7" s="5">
+        <v>10</v>
+      </c>
+      <c r="I7" s="101"/>
       <c r="J7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K7" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="37"/>
+      <c r="M7" s="73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15" customHeight="1">
+      <c r="A8" s="98"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="68">
+      <c r="E8" s="7">
         <v>9</v>
       </c>
-      <c r="I8" s="44"/>
+      <c r="I8" s="101"/>
       <c r="J8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="K8" s="6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="57">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="37"/>
+      <c r="M8" s="72">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15" customHeight="1">
+      <c r="A9" s="98"/>
       <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="69">
-        <v>10</v>
-      </c>
-      <c r="I9" s="44"/>
+      <c r="E9" s="5">
+        <v>11</v>
+      </c>
+      <c r="I9" s="101"/>
       <c r="J9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K9" s="8">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M9" s="58">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="40"/>
+      <c r="M9" s="73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15" customHeight="1" thickBot="1">
+      <c r="A10" s="99"/>
       <c r="B10" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="10">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="70">
-        <v>8</v>
-      </c>
-      <c r="I10" s="45"/>
+      <c r="E10" s="10">
+        <v>14</v>
+      </c>
+      <c r="I10" s="102"/>
       <c r="J10" s="10" t="s">
         <v>16</v>
       </c>
       <c r="K10" s="9">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M10" s="59">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="41">
-        <v>2022</v>
+      <c r="M10" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A11" s="97">
+        <v>2020</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="67">
+      <c r="E11" s="3">
+        <v>5</v>
+      </c>
+      <c r="I11" s="100">
+        <v>2020</v>
+      </c>
+      <c r="J11" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="76">
+        <v>2</v>
+      </c>
+      <c r="L11" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="46">
-        <v>2022</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K11" s="4">
-        <v>5</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M11" s="56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="37"/>
+      <c r="M11" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15" customHeight="1">
+      <c r="A12" s="98"/>
       <c r="B12" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="7">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="68">
-        <v>17</v>
-      </c>
-      <c r="I12" s="44"/>
+      <c r="E12" s="7">
+        <v>13</v>
+      </c>
+      <c r="I12" s="101"/>
       <c r="J12" s="7" t="s">
         <v>8</v>
       </c>
       <c r="K12" s="6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M12" s="57">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="37"/>
+      <c r="M12" s="72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15" customHeight="1">
+      <c r="A13" s="98"/>
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="5">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="69">
-        <v>13</v>
-      </c>
-      <c r="I13" s="44"/>
+      <c r="E13" s="5">
+        <v>14</v>
+      </c>
+      <c r="I13" s="101"/>
       <c r="J13" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K13" s="8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M13" s="58">
+      <c r="M13" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="37"/>
+    <row r="14" spans="1:13" ht="15" customHeight="1">
+      <c r="A14" s="98"/>
       <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="7">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="68">
-        <v>15</v>
-      </c>
-      <c r="I14" s="44"/>
+      <c r="E14" s="7">
+        <v>19</v>
+      </c>
+      <c r="I14" s="101"/>
       <c r="J14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="K14" s="6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M14" s="57">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="37"/>
+      <c r="M14" s="72">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15" customHeight="1">
+      <c r="A15" s="98"/>
       <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="5">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="69">
-        <v>12</v>
-      </c>
-      <c r="I15" s="44"/>
+      <c r="E15" s="5">
+        <v>9</v>
+      </c>
+      <c r="I15" s="101"/>
       <c r="J15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K15" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="38"/>
+      <c r="M15" s="73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15" customHeight="1" thickBot="1">
+      <c r="A16" s="99"/>
       <c r="B16" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="10">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="70">
-        <v>20</v>
-      </c>
-      <c r="I16" s="45"/>
+      <c r="E16" s="10">
+        <v>9</v>
+      </c>
+      <c r="I16" s="102"/>
       <c r="J16" s="10" t="s">
         <v>16</v>
       </c>
       <c r="K16" s="9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M16" s="59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="37">
-        <v>2023</v>
+      <c r="M16" s="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15" thickTop="1">
+      <c r="A17" s="95">
+        <v>2021</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="3">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="67">
-        <v>9</v>
-      </c>
-      <c r="I17" s="46">
-        <v>2023</v>
+      <c r="E17" s="46">
+        <v>17</v>
+      </c>
+      <c r="I17" s="91">
+        <v>2021</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>6</v>
@@ -2162,459 +2308,819 @@
       <c r="L17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="60">
-        <v>0</v>
+      <c r="M17" s="35">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="37"/>
+      <c r="A18" s="92"/>
       <c r="B18" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="68">
-        <v>9</v>
-      </c>
-      <c r="I18" s="44"/>
+      <c r="E18" s="47">
+        <v>13</v>
+      </c>
+      <c r="I18" s="86"/>
       <c r="J18" s="7" t="s">
         <v>8</v>
       </c>
       <c r="K18" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M18" s="57">
-        <v>1</v>
+      <c r="M18" s="36">
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="37"/>
+      <c r="A19" s="92"/>
       <c r="B19" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="69">
-        <v>13</v>
-      </c>
-      <c r="I19" s="44"/>
+      <c r="E19" s="48">
+        <v>7</v>
+      </c>
+      <c r="I19" s="86"/>
       <c r="J19" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K19" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M19" s="60">
-        <v>12</v>
+      <c r="M19" s="37">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="37"/>
+      <c r="A20" s="92"/>
       <c r="B20" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="68">
-        <v>11</v>
-      </c>
-      <c r="I20" s="44"/>
+      <c r="E20" s="47">
+        <v>9</v>
+      </c>
+      <c r="I20" s="86"/>
       <c r="J20" s="7" t="s">
         <v>12</v>
       </c>
       <c r="K20" s="6">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M20" s="57">
-        <v>1</v>
+      <c r="M20" s="36">
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="37"/>
+      <c r="A21" s="92"/>
       <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="5">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="69">
-        <v>15</v>
-      </c>
-      <c r="I21" s="44"/>
+      <c r="E21" s="48">
+        <v>10</v>
+      </c>
+      <c r="I21" s="86"/>
       <c r="J21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="15">
-        <v>1</v>
+      <c r="K21" s="8">
+        <v>0</v>
       </c>
       <c r="L21" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M21" s="60">
+      <c r="M21" s="37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="96"/>
+      <c r="B22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="10">
+        <v>26</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="49">
+        <v>8</v>
+      </c>
+      <c r="I22" s="90"/>
+      <c r="J22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="9">
+        <v>13</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M22" s="38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="94">
+        <v>2022</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="3">
+        <v>14</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="46">
+        <v>7</v>
+      </c>
+      <c r="I23" s="85">
+        <v>2022</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="4">
+        <v>5</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M23" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="92"/>
+      <c r="B24" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="7">
+        <v>8</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="47">
+        <v>17</v>
+      </c>
+      <c r="I24" s="86"/>
+      <c r="J24" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" s="6">
+        <v>1</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M24" s="36">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="38"/>
-      <c r="B22" s="28" t="s">
+    <row r="25" spans="1:13">
+      <c r="A25" s="92"/>
+      <c r="B25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="5">
+        <v>19</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="48">
+        <v>13</v>
+      </c>
+      <c r="I25" s="86"/>
+      <c r="J25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K25" s="8">
+        <v>4</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M25" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="92"/>
+      <c r="B26" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="7">
+        <v>9</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="47">
+        <v>15</v>
+      </c>
+      <c r="I26" s="86"/>
+      <c r="J26" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K26" s="6">
+        <v>3</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M26" s="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="92"/>
+      <c r="B27" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="5">
+        <v>21</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="48">
+        <v>12</v>
+      </c>
+      <c r="I27" s="86"/>
+      <c r="J27" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K27" s="8">
+        <v>5</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M27" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="93"/>
+      <c r="B28" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C28" s="10">
+        <v>14</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="49">
+        <v>20</v>
+      </c>
+      <c r="I28" s="90"/>
+      <c r="J28" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" s="9">
+        <v>3</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M28" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="92">
+        <v>2023</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="3">
+        <v>6</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="46">
+        <v>9</v>
+      </c>
+      <c r="I29" s="85">
+        <v>2023</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K29" s="4">
+        <v>1</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M29" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="92"/>
+      <c r="B30" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="7">
+        <v>11</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="47">
+        <v>9</v>
+      </c>
+      <c r="I30" s="86"/>
+      <c r="J30" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K30" s="6">
+        <v>0</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M30" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="92"/>
+      <c r="B31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="5">
+        <v>9</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="48">
+        <v>13</v>
+      </c>
+      <c r="I31" s="86"/>
+      <c r="J31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K31" s="8">
+        <v>3</v>
+      </c>
+      <c r="L31" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M31" s="39">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="92"/>
+      <c r="B32" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="7">
+        <v>10</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="47">
+        <v>11</v>
+      </c>
+      <c r="I32" s="86"/>
+      <c r="J32" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K32" s="6">
+        <v>1</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M32" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="92"/>
+      <c r="B33" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="5">
+        <v>17</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="48">
+        <v>16</v>
+      </c>
+      <c r="I33" s="86"/>
+      <c r="J33" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K33" s="15">
+        <v>1</v>
+      </c>
+      <c r="L33" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M33" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="93"/>
+      <c r="B34" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="20">
         <v>23</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D34" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="71">
+      <c r="E34" s="50">
         <v>11</v>
       </c>
-      <c r="I22" s="45"/>
-      <c r="J22" s="28" t="s">
+      <c r="I34" s="90"/>
+      <c r="J34" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="K22" s="29">
+      <c r="K34" s="21">
         <v>8</v>
       </c>
-      <c r="L22" s="29" t="s">
+      <c r="L34" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="M22" s="61">
+      <c r="M34" s="40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="82">
+        <v>2024</v>
+      </c>
+      <c r="B35" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="29">
+        <v>12</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="41">
+        <v>20</v>
+      </c>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="85">
+        <v>2024</v>
+      </c>
+      <c r="J35" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="K35" s="29">
+        <v>1</v>
+      </c>
+      <c r="L35" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="M35" s="41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="83"/>
+      <c r="B36" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="18">
+        <v>11</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="42">
+        <v>15</v>
+      </c>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="86"/>
+      <c r="J36" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="K36" s="18">
+        <v>1</v>
+      </c>
+      <c r="L36" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="M36" s="42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="83"/>
+      <c r="B37" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="18">
+        <v>17</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="42">
+        <v>15</v>
+      </c>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="86"/>
+      <c r="J37" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="K37" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="39">
+      <c r="L37" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="M37" s="42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="83"/>
+      <c r="B38" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="18">
+        <v>13</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="42">
+        <v>20</v>
+      </c>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="86"/>
+      <c r="J38" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="K38" s="18">
+        <v>1</v>
+      </c>
+      <c r="L38" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M38" s="42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="83"/>
+      <c r="B39" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="18">
+        <v>18</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="42">
+        <v>16</v>
+      </c>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="86"/>
+      <c r="J39" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="K39" s="18">
+        <v>2</v>
+      </c>
+      <c r="L39" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M39" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="84"/>
+      <c r="B40" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="33">
+        <v>14</v>
+      </c>
+      <c r="D40" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="43">
+        <v>11</v>
+      </c>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="87"/>
+      <c r="J40" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="33">
+        <v>2</v>
+      </c>
+      <c r="L40" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="M40" s="43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="15">
+      <c r="A42" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="J42" s="69" t="s">
+        <v>19</v>
+      </c>
+      <c r="M42" s="28"/>
+    </row>
+    <row r="43" spans="1:13" ht="21" customHeight="1">
+      <c r="A43" s="59">
+        <v>2019</v>
+      </c>
+      <c r="B43" s="53">
+        <v>143</v>
+      </c>
+      <c r="I43" s="65">
+        <v>2019</v>
+      </c>
+      <c r="J43" s="53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="15">
+      <c r="A44" s="60">
+        <v>2020</v>
+      </c>
+      <c r="B44" s="54">
+        <v>128</v>
+      </c>
+      <c r="I44" s="66">
+        <v>2020</v>
+      </c>
+      <c r="J44" s="54">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="15">
+      <c r="A45" s="61">
+        <v>2021</v>
+      </c>
+      <c r="B45" s="55">
+        <v>141</v>
+      </c>
+      <c r="F45" s="28"/>
+      <c r="I45" s="67">
+        <v>2021</v>
+      </c>
+      <c r="J45" s="55">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="15">
+      <c r="A46" s="62">
+        <v>2022</v>
+      </c>
+      <c r="B46" s="56">
+        <v>169</v>
+      </c>
+      <c r="F46" s="28"/>
+      <c r="I46" s="68">
+        <v>2022</v>
+      </c>
+      <c r="J46" s="56">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="15">
+      <c r="A47" s="63">
+        <v>2023</v>
+      </c>
+      <c r="B47" s="57">
+        <v>145</v>
+      </c>
+      <c r="F47" s="28"/>
+      <c r="I47" s="68">
+        <v>2023</v>
+      </c>
+      <c r="J47" s="56">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="15">
+      <c r="A48" s="63">
         <v>2024</v>
       </c>
-      <c r="B23" s="65" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="50">
-        <v>12</v>
-      </c>
-      <c r="D23" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="62">
+      <c r="B48" s="55">
+        <v>182</v>
+      </c>
+      <c r="F48" s="28"/>
+      <c r="I48" s="68">
+        <v>2024</v>
+      </c>
+      <c r="J48" s="56">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="46">
-        <v>2024</v>
-      </c>
-      <c r="J23" s="52" t="s">
-        <v>6</v>
-      </c>
-      <c r="K23" s="50">
-        <v>1</v>
-      </c>
-      <c r="L23" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="M23" s="62">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="32"/>
-      <c r="B24" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="26">
-        <v>11</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="63">
-        <v>14</v>
-      </c>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="K24" s="26">
-        <v>0</v>
-      </c>
-      <c r="L24" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="M24" s="63">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="32"/>
-      <c r="B25" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="26">
-        <v>17</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="63">
-        <v>15</v>
-      </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K25" s="26">
-        <v>0</v>
-      </c>
-      <c r="L25" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="M25" s="63">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="32"/>
-      <c r="B26" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="26">
-        <v>12</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="63">
-        <v>19</v>
-      </c>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="K26" s="26">
-        <v>1</v>
-      </c>
-      <c r="L26" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="M26" s="63">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="32"/>
-      <c r="B27" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="26">
-        <v>17</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="63"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="K27" s="26">
-        <v>2</v>
-      </c>
-      <c r="L27" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="M27" s="63"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="33"/>
-      <c r="B28" s="66" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="54">
-        <v>14</v>
-      </c>
-      <c r="D28" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="64"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="K28" s="54">
-        <v>2</v>
-      </c>
-      <c r="L28" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="M28" s="64"/>
-    </row>
-    <row r="30" spans="1:13" ht="30">
-      <c r="A30" s="72" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="91" t="s">
-        <v>18</v>
-      </c>
-      <c r="I30" s="73" t="s">
-        <v>3</v>
-      </c>
-      <c r="J30" s="90" t="s">
-        <v>19</v>
-      </c>
-      <c r="M30" s="49"/>
-    </row>
-    <row r="31" spans="1:13" ht="21" customHeight="1">
-      <c r="A31" s="80">
-        <v>2019</v>
-      </c>
-      <c r="B31" s="74">
-        <v>143</v>
-      </c>
-      <c r="I31" s="86">
-        <v>2019</v>
-      </c>
-      <c r="J31" s="74">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="81">
-        <v>2020</v>
-      </c>
-      <c r="B32" s="75">
-        <v>128</v>
-      </c>
-      <c r="I32" s="87">
-        <v>2020</v>
-      </c>
-      <c r="J32" s="75">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="82">
-        <v>2021</v>
-      </c>
-      <c r="B33" s="76">
-        <v>139</v>
-      </c>
-      <c r="F33" s="49"/>
-      <c r="I33" s="88">
-        <v>2021</v>
-      </c>
-      <c r="J33" s="76">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="83">
-        <v>2022</v>
-      </c>
-      <c r="B34" s="77">
-        <v>169</v>
-      </c>
-      <c r="F34" s="49"/>
-      <c r="I34" s="89">
-        <v>2022</v>
-      </c>
-      <c r="J34" s="77">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="84">
-        <v>2023</v>
-      </c>
-      <c r="B35" s="78">
-        <v>144</v>
-      </c>
-      <c r="F35" s="49"/>
-      <c r="I35" s="89">
-        <v>2023</v>
-      </c>
-      <c r="J35" s="77">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="84">
-        <v>2024</v>
-      </c>
-      <c r="B36" s="76"/>
-      <c r="F36" s="49"/>
-      <c r="I36" s="89">
-        <v>2024</v>
-      </c>
-      <c r="J36" s="77"/>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="85" t="s">
+      <c r="B49" s="58">
+        <v>908</v>
+      </c>
+      <c r="F49" s="28"/>
+      <c r="I49" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="79">
-        <v>723</v>
-      </c>
-      <c r="F37" s="49"/>
-      <c r="I37" s="85" t="s">
-        <v>20</v>
-      </c>
-      <c r="J37" s="79">
-        <v>196</v>
+      <c r="J49" s="58">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="I23:I28"/>
+  <mergeCells count="15">
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="I35:I40"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="I3:M3"/>
+    <mergeCell ref="I29:I34"/>
     <mergeCell ref="I17:I22"/>
-    <mergeCell ref="I5:I10"/>
-    <mergeCell ref="I11:I16"/>
+    <mergeCell ref="I23:I28"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A23:A28"/>
     <mergeCell ref="A17:A22"/>
     <mergeCell ref="A11:A16"/>
     <mergeCell ref="A5:A10"/>
+    <mergeCell ref="I5:I10"/>
+    <mergeCell ref="I11:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -2625,90 +3131,204 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6640C042-80F5-4BF7-8065-A32AA286BAD5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="30.75">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:3" ht="29.25" thickBot="1">
+      <c r="A1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="79" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="21">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1">
+      <c r="A2" s="59">
         <v>2019</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="53">
         <v>143</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15">
+      <c r="A3" s="60">
+        <v>2020</v>
+      </c>
+      <c r="B3" s="54">
+        <v>128</v>
+      </c>
+      <c r="C3" s="54">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15">
+      <c r="A4" s="61">
+        <v>2021</v>
+      </c>
+      <c r="B4" s="55">
+        <v>141</v>
+      </c>
+      <c r="C4" s="55">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15">
+      <c r="A5" s="62">
+        <v>2022</v>
+      </c>
+      <c r="B5" s="56">
+        <v>169</v>
+      </c>
+      <c r="C5" s="56">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15">
+      <c r="A6" s="63">
+        <v>2023</v>
+      </c>
+      <c r="B6" s="57">
+        <v>145</v>
+      </c>
+      <c r="C6" s="56">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15">
+      <c r="A7" s="62">
+        <v>2024</v>
+      </c>
+      <c r="B7" s="81">
+        <v>182</v>
+      </c>
+      <c r="C7" s="56">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="80" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="80" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="80" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="80" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>2019</v>
+      </c>
+      <c r="B2">
+        <v>51</v>
+      </c>
+      <c r="C2">
+        <v>92</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2020</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>78</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>2021</v>
+      </c>
+      <c r="B4">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="21">
-        <v>2020</v>
-      </c>
-      <c r="B3" s="22">
-        <v>128</v>
-      </c>
-      <c r="C3" s="22">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="21">
-        <v>2021</v>
-      </c>
-      <c r="B4" s="22">
-        <v>139</v>
-      </c>
-      <c r="C4" s="22">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="21">
+      <c r="C4">
+        <v>88</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
         <v>2022</v>
       </c>
-      <c r="B5" s="22">
-        <v>169</v>
-      </c>
-      <c r="C5" s="22">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="21">
+      <c r="B5">
+        <v>71</v>
+      </c>
+      <c r="C5">
+        <v>98</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
         <v>2023</v>
       </c>
-      <c r="B6" s="22">
-        <v>144</v>
-      </c>
-      <c r="C6" s="22">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="21">
+      <c r="B6">
+        <v>67</v>
+      </c>
+      <c r="C6">
+        <v>77</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
         <v>2024</v>
       </c>
-      <c r="B7" s="23">
-        <v>151</v>
-      </c>
-      <c r="C7" s="23">
-        <v>21</v>
+      <c r="B7">
+        <v>94</v>
+      </c>
+      <c r="C7">
+        <v>88</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new tab to CAVV and update data for the other tabs in CAVV
</commit_message>
<xml_diff>
--- a/data/Prevencion_de_violencia_de_genero_CAVV/SAFEkits.xlsx
+++ b/data/Prevencion_de_violencia_de_genero_CAVV/SAFEkits.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlando.hernandez\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnper\Documents\ViolenciaGeneroPR\data\Prevencion_de_violencia_de_genero_CAVV\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E38751-0D19-4A42-865F-0C5E83C2384B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="Edades" sheetId="3" r:id="rId3"/>
+    <sheet name="Kit Analizados" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="27">
   <si>
     <t>Equipo de recolección de evidencia en casos de violencia sexual (RAPE kits/ SAFE Kits)</t>
   </si>
@@ -110,12 +112,21 @@
   <si>
     <t>No identificado</t>
   </si>
+  <si>
+    <t>Laboratorio Forense</t>
+  </si>
+  <si>
+    <t>Laboratorios Externos: BODE</t>
+  </si>
+  <si>
+    <t>Laboratorios Externos: DNA Solutions</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +179,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -203,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="61">
+  <borders count="73">
     <border>
       <left/>
       <right/>
@@ -862,19 +880,6 @@
       <left style="thick">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
       <right style="thick">
         <color rgb="FF000000"/>
       </right>
@@ -1001,6 +1006,185 @@
       </right>
       <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1009,7 +1193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1059,10 +1243,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1090,10 +1270,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1103,7 +1279,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1127,13 +1303,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1178,9 +1354,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1195,9 +1368,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1217,25 +1387,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1247,7 +1417,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1295,13 +1465,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1310,14 +1483,126 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thick">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1422,70 +1707,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="medium">
           <color indexed="64"/>
@@ -1516,22 +1737,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A42:B48" totalsRowShown="0" headerRowBorderDxfId="8" tableBorderDxfId="7">
-  <autoFilter ref="A42:B48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A48:B55" totalsRowShown="0" headerRowBorderDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="A48:B55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Año" dataDxfId="6"/>
-    <tableColumn id="2" name="Total con querella" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Año" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Total con querella" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="I42:J49" totalsRowShown="0" dataDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="2">
-  <autoFilter ref="I42:J49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="I48:J56" totalsRowShown="0" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
+  <autoFilter ref="I48:J56" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Año" dataDxfId="1"/>
-    <tableColumn id="2" name="Total sin querella" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Año" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Total sin querella" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1853,59 +2074,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M1"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.375" customWidth="1"/>
-    <col min="2" max="2" width="16.875" customWidth="1"/>
-    <col min="3" max="3" width="13.375" customWidth="1"/>
-    <col min="4" max="4" width="14.75" customWidth="1"/>
-    <col min="5" max="5" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="12" max="12" width="13.375" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18">
-      <c r="A1" s="88" t="s">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-    </row>
-    <row r="3" spans="1:13" ht="20.25">
-      <c r="A3" s="89" t="s">
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+    </row>
+    <row r="3" spans="1:13" ht="21" x14ac:dyDescent="0.4">
+      <c r="A3" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="I3" s="89" t="s">
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="I3" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-    </row>
-    <row r="4" spans="1:13" ht="30.75" thickBot="1">
-      <c r="A4" s="26" t="s">
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+    </row>
+    <row r="4" spans="1:13" ht="31.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="24" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1920,7 +2141,7 @@
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="25" t="s">
         <v>3</v>
       </c>
       <c r="J4" s="13" t="s">
@@ -1936,8 +2157,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A5" s="97">
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="91">
         <v>2019</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1952,7 +2173,7 @@
       <c r="E5" s="3">
         <v>14</v>
       </c>
-      <c r="I5" s="100">
+      <c r="I5" s="94">
         <v>2019</v>
       </c>
       <c r="J5" s="3" t="s">
@@ -1964,12 +2185,12 @@
       <c r="L5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="71">
+      <c r="M5" s="65">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" customHeight="1">
-      <c r="A6" s="98"/>
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="92"/>
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
@@ -1982,7 +2203,7 @@
       <c r="E6" s="7">
         <v>13</v>
       </c>
-      <c r="I6" s="101"/>
+      <c r="I6" s="95"/>
       <c r="J6" s="7" t="s">
         <v>8</v>
       </c>
@@ -1992,12 +2213,12 @@
       <c r="L6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="72">
+      <c r="M6" s="66">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" customHeight="1">
-      <c r="A7" s="98"/>
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="92"/>
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -2010,7 +2231,7 @@
       <c r="E7" s="5">
         <v>10</v>
       </c>
-      <c r="I7" s="101"/>
+      <c r="I7" s="95"/>
       <c r="J7" s="5" t="s">
         <v>10</v>
       </c>
@@ -2020,12 +2241,12 @@
       <c r="L7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="73">
+      <c r="M7" s="67">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1">
-      <c r="A8" s="98"/>
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="92"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2038,7 +2259,7 @@
       <c r="E8" s="7">
         <v>9</v>
       </c>
-      <c r="I8" s="101"/>
+      <c r="I8" s="95"/>
       <c r="J8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2048,12 +2269,12 @@
       <c r="L8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="72">
+      <c r="M8" s="66">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1">
-      <c r="A9" s="98"/>
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="92"/>
       <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
@@ -2066,7 +2287,7 @@
       <c r="E9" s="5">
         <v>11</v>
       </c>
-      <c r="I9" s="101"/>
+      <c r="I9" s="95"/>
       <c r="J9" s="5" t="s">
         <v>14</v>
       </c>
@@ -2076,12 +2297,12 @@
       <c r="L9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M9" s="73">
+      <c r="M9" s="67">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1" thickBot="1">
-      <c r="A10" s="99"/>
+    <row r="10" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="93"/>
       <c r="B10" s="10" t="s">
         <v>16</v>
       </c>
@@ -2094,7 +2315,7 @@
       <c r="E10" s="10">
         <v>14</v>
       </c>
-      <c r="I10" s="102"/>
+      <c r="I10" s="96"/>
       <c r="J10" s="10" t="s">
         <v>16</v>
       </c>
@@ -2104,12 +2325,12 @@
       <c r="L10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M10" s="74">
+      <c r="M10" s="68">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A11" s="97">
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="91">
         <v>2020</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2124,24 +2345,24 @@
       <c r="E11" s="3">
         <v>5</v>
       </c>
-      <c r="I11" s="100">
+      <c r="I11" s="94">
         <v>2020</v>
       </c>
-      <c r="J11" s="75" t="s">
+      <c r="J11" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="76">
+      <c r="K11" s="70">
         <v>2</v>
       </c>
-      <c r="L11" s="76" t="s">
+      <c r="L11" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="77">
+      <c r="M11" s="71">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1">
-      <c r="A12" s="98"/>
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="92"/>
       <c r="B12" s="7" t="s">
         <v>8</v>
       </c>
@@ -2154,7 +2375,7 @@
       <c r="E12" s="7">
         <v>13</v>
       </c>
-      <c r="I12" s="101"/>
+      <c r="I12" s="95"/>
       <c r="J12" s="7" t="s">
         <v>8</v>
       </c>
@@ -2164,12 +2385,12 @@
       <c r="L12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M12" s="72">
+      <c r="M12" s="66">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1">
-      <c r="A13" s="98"/>
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="92"/>
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
@@ -2182,7 +2403,7 @@
       <c r="E13" s="5">
         <v>14</v>
       </c>
-      <c r="I13" s="101"/>
+      <c r="I13" s="95"/>
       <c r="J13" s="5" t="s">
         <v>10</v>
       </c>
@@ -2192,12 +2413,12 @@
       <c r="L13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M13" s="73">
+      <c r="M13" s="67">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1">
-      <c r="A14" s="98"/>
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="92"/>
       <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
@@ -2210,7 +2431,7 @@
       <c r="E14" s="7">
         <v>19</v>
       </c>
-      <c r="I14" s="101"/>
+      <c r="I14" s="95"/>
       <c r="J14" s="7" t="s">
         <v>12</v>
       </c>
@@ -2220,12 +2441,12 @@
       <c r="L14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M14" s="72">
+      <c r="M14" s="66">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1">
-      <c r="A15" s="98"/>
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="92"/>
       <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
@@ -2238,7 +2459,7 @@
       <c r="E15" s="5">
         <v>9</v>
       </c>
-      <c r="I15" s="101"/>
+      <c r="I15" s="95"/>
       <c r="J15" s="5" t="s">
         <v>14</v>
       </c>
@@ -2248,12 +2469,12 @@
       <c r="L15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="73">
+      <c r="M15" s="67">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" thickBot="1">
-      <c r="A16" s="99"/>
+    <row r="16" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="93"/>
       <c r="B16" s="10" t="s">
         <v>16</v>
       </c>
@@ -2266,7 +2487,7 @@
       <c r="E16" s="10">
         <v>9</v>
       </c>
-      <c r="I16" s="102"/>
+      <c r="I16" s="96"/>
       <c r="J16" s="10" t="s">
         <v>16</v>
       </c>
@@ -2276,12 +2497,12 @@
       <c r="L16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M16" s="74">
+      <c r="M16" s="68">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15" thickTop="1">
-      <c r="A17" s="95">
+    <row r="17" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="89">
         <v>2021</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -2293,10 +2514,10 @@
       <c r="D17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="46">
-        <v>17</v>
-      </c>
-      <c r="I17" s="91">
+      <c r="E17" s="42">
+        <v>15</v>
+      </c>
+      <c r="I17" s="85">
         <v>2021</v>
       </c>
       <c r="J17" s="3" t="s">
@@ -2308,12 +2529,12 @@
       <c r="L17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="35">
+      <c r="M17" s="31">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="92"/>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="86"/>
       <c r="B18" s="7" t="s">
         <v>8</v>
       </c>
@@ -2323,10 +2544,10 @@
       <c r="D18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="47">
+      <c r="E18" s="43">
         <v>13</v>
       </c>
-      <c r="I18" s="86"/>
+      <c r="I18" s="80"/>
       <c r="J18" s="7" t="s">
         <v>8</v>
       </c>
@@ -2336,12 +2557,12 @@
       <c r="L18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M18" s="36">
+      <c r="M18" s="32">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="92"/>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="86"/>
       <c r="B19" s="5" t="s">
         <v>10</v>
       </c>
@@ -2351,10 +2572,10 @@
       <c r="D19" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="48">
+      <c r="E19" s="44">
         <v>7</v>
       </c>
-      <c r="I19" s="86"/>
+      <c r="I19" s="80"/>
       <c r="J19" s="5" t="s">
         <v>10</v>
       </c>
@@ -2364,12 +2585,12 @@
       <c r="L19" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M19" s="37">
+      <c r="M19" s="33">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="92"/>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="86"/>
       <c r="B20" s="7" t="s">
         <v>12</v>
       </c>
@@ -2379,10 +2600,10 @@
       <c r="D20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="47">
+      <c r="E20" s="43">
         <v>9</v>
       </c>
-      <c r="I20" s="86"/>
+      <c r="I20" s="80"/>
       <c r="J20" s="7" t="s">
         <v>12</v>
       </c>
@@ -2392,12 +2613,12 @@
       <c r="L20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M20" s="36">
+      <c r="M20" s="32">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="92"/>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="86"/>
       <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
@@ -2407,10 +2628,10 @@
       <c r="D21" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="48">
+      <c r="E21" s="44">
         <v>10</v>
       </c>
-      <c r="I21" s="86"/>
+      <c r="I21" s="80"/>
       <c r="J21" s="5" t="s">
         <v>14</v>
       </c>
@@ -2420,12 +2641,12 @@
       <c r="L21" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M21" s="37">
+      <c r="M21" s="33">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="96"/>
+    <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="90"/>
       <c r="B22" s="10" t="s">
         <v>16</v>
       </c>
@@ -2435,10 +2656,10 @@
       <c r="D22" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="49">
+      <c r="E22" s="45">
         <v>8</v>
       </c>
-      <c r="I22" s="90"/>
+      <c r="I22" s="84"/>
       <c r="J22" s="10" t="s">
         <v>16</v>
       </c>
@@ -2448,12 +2669,12 @@
       <c r="L22" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M22" s="38">
+      <c r="M22" s="34">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="94">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="88">
         <v>2022</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -2465,10 +2686,10 @@
       <c r="D23" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="46">
+      <c r="E23" s="42">
         <v>7</v>
       </c>
-      <c r="I23" s="85">
+      <c r="I23" s="79">
         <v>2022</v>
       </c>
       <c r="J23" s="3" t="s">
@@ -2480,12 +2701,12 @@
       <c r="L23" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M23" s="35">
+      <c r="M23" s="31">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="92"/>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="86"/>
       <c r="B24" s="7" t="s">
         <v>8</v>
       </c>
@@ -2495,10 +2716,10 @@
       <c r="D24" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="47">
+      <c r="E24" s="43">
         <v>17</v>
       </c>
-      <c r="I24" s="86"/>
+      <c r="I24" s="80"/>
       <c r="J24" s="7" t="s">
         <v>8</v>
       </c>
@@ -2508,12 +2729,12 @@
       <c r="L24" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M24" s="36">
+      <c r="M24" s="32">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
-      <c r="A25" s="92"/>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="86"/>
       <c r="B25" s="5" t="s">
         <v>10</v>
       </c>
@@ -2523,10 +2744,10 @@
       <c r="D25" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="48">
+      <c r="E25" s="44">
         <v>13</v>
       </c>
-      <c r="I25" s="86"/>
+      <c r="I25" s="80"/>
       <c r="J25" s="5" t="s">
         <v>10</v>
       </c>
@@ -2536,12 +2757,12 @@
       <c r="L25" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M25" s="37">
+      <c r="M25" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
-      <c r="A26" s="92"/>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="86"/>
       <c r="B26" s="7" t="s">
         <v>12</v>
       </c>
@@ -2551,10 +2772,10 @@
       <c r="D26" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="47">
+      <c r="E26" s="43">
         <v>15</v>
       </c>
-      <c r="I26" s="86"/>
+      <c r="I26" s="80"/>
       <c r="J26" s="7" t="s">
         <v>12</v>
       </c>
@@ -2564,12 +2785,12 @@
       <c r="L26" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M26" s="36">
+      <c r="M26" s="32">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
-      <c r="A27" s="92"/>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="86"/>
       <c r="B27" s="5" t="s">
         <v>14</v>
       </c>
@@ -2579,10 +2800,10 @@
       <c r="D27" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="48">
+      <c r="E27" s="44">
         <v>12</v>
       </c>
-      <c r="I27" s="86"/>
+      <c r="I27" s="80"/>
       <c r="J27" s="5" t="s">
         <v>14</v>
       </c>
@@ -2592,12 +2813,12 @@
       <c r="L27" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="37">
+      <c r="M27" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="93"/>
+    <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="87"/>
       <c r="B28" s="10" t="s">
         <v>16</v>
       </c>
@@ -2607,10 +2828,10 @@
       <c r="D28" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E28" s="49">
+      <c r="E28" s="45">
         <v>20</v>
       </c>
-      <c r="I28" s="90"/>
+      <c r="I28" s="84"/>
       <c r="J28" s="10" t="s">
         <v>16</v>
       </c>
@@ -2620,12 +2841,12 @@
       <c r="L28" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M28" s="38">
+      <c r="M28" s="34">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="92">
+    <row r="29" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="86">
         <v>2023</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -2637,10 +2858,10 @@
       <c r="D29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="46">
+      <c r="E29" s="42">
         <v>9</v>
       </c>
-      <c r="I29" s="85">
+      <c r="I29" s="79">
         <v>2023</v>
       </c>
       <c r="J29" s="3" t="s">
@@ -2652,12 +2873,12 @@
       <c r="L29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M29" s="39">
+      <c r="M29" s="35">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="92"/>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="86"/>
       <c r="B30" s="7" t="s">
         <v>8</v>
       </c>
@@ -2667,10 +2888,10 @@
       <c r="D30" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="47">
+      <c r="E30" s="43">
         <v>9</v>
       </c>
-      <c r="I30" s="86"/>
+      <c r="I30" s="80"/>
       <c r="J30" s="7" t="s">
         <v>8</v>
       </c>
@@ -2680,12 +2901,12 @@
       <c r="L30" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M30" s="36">
+      <c r="M30" s="32">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="92"/>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="86"/>
       <c r="B31" s="5" t="s">
         <v>10</v>
       </c>
@@ -2695,10 +2916,10 @@
       <c r="D31" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="48">
+      <c r="E31" s="44">
         <v>13</v>
       </c>
-      <c r="I31" s="86"/>
+      <c r="I31" s="80"/>
       <c r="J31" s="5" t="s">
         <v>10</v>
       </c>
@@ -2708,12 +2929,12 @@
       <c r="L31" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M31" s="39">
+      <c r="M31" s="35">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="92"/>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="86"/>
       <c r="B32" s="7" t="s">
         <v>12</v>
       </c>
@@ -2723,10 +2944,10 @@
       <c r="D32" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="47">
+      <c r="E32" s="43">
         <v>11</v>
       </c>
-      <c r="I32" s="86"/>
+      <c r="I32" s="80"/>
       <c r="J32" s="7" t="s">
         <v>12</v>
       </c>
@@ -2736,12 +2957,12 @@
       <c r="L32" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M32" s="36">
+      <c r="M32" s="32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="92"/>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="86"/>
       <c r="B33" s="5" t="s">
         <v>14</v>
       </c>
@@ -2751,10 +2972,10 @@
       <c r="D33" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="48">
-        <v>16</v>
-      </c>
-      <c r="I33" s="86"/>
+      <c r="E33" s="44">
+        <v>15</v>
+      </c>
+      <c r="I33" s="80"/>
       <c r="J33" s="5" t="s">
         <v>14</v>
       </c>
@@ -2764,348 +2985,487 @@
       <c r="L33" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M33" s="39">
+      <c r="M33" s="35">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="93"/>
-      <c r="B34" s="20" t="s">
+    <row r="34" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="87"/>
+      <c r="B34" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="20">
+      <c r="C34" s="18">
         <v>23</v>
       </c>
-      <c r="D34" s="21" t="s">
+      <c r="D34" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E34" s="50">
+      <c r="E34" s="46">
         <v>11</v>
       </c>
-      <c r="I34" s="90"/>
-      <c r="J34" s="20" t="s">
+      <c r="I34" s="84"/>
+      <c r="J34" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="K34" s="21">
+      <c r="K34" s="19">
         <v>8</v>
       </c>
-      <c r="L34" s="21" t="s">
+      <c r="L34" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="M34" s="40">
+      <c r="M34" s="36">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="82">
+    <row r="35" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="76">
         <v>2024</v>
       </c>
-      <c r="B35" s="44" t="s">
+      <c r="B35" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="29">
+      <c r="C35" s="26">
         <v>12</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="D35" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="37">
         <v>20</v>
       </c>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="85">
+      <c r="I35" s="79">
         <v>2024</v>
       </c>
-      <c r="J35" s="31" t="s">
+      <c r="J35" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="K35" s="29">
+      <c r="K35" s="26">
         <v>1</v>
       </c>
-      <c r="L35" s="30" t="s">
+      <c r="L35" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="M35" s="41">
+      <c r="M35" s="37">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="83"/>
-      <c r="B36" s="25" t="s">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="77"/>
+      <c r="B36" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="18">
+      <c r="C36" s="16">
         <v>11</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E36" s="42">
+      <c r="E36" s="38">
         <v>15</v>
       </c>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="86"/>
-      <c r="J36" s="22" t="s">
+      <c r="I36" s="80"/>
+      <c r="J36" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="K36" s="18">
+      <c r="K36" s="16">
         <v>1</v>
       </c>
-      <c r="L36" s="19" t="s">
+      <c r="L36" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="M36" s="42">
+      <c r="M36" s="38">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="83"/>
-      <c r="B37" s="24" t="s">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="77"/>
+      <c r="B37" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="18">
+      <c r="C37" s="16">
         <v>17</v>
       </c>
       <c r="D37" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="42">
+      <c r="E37" s="38">
         <v>15</v>
       </c>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="86"/>
-      <c r="J37" s="23" t="s">
+      <c r="I37" s="80"/>
+      <c r="J37" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="K37" s="18">
+      <c r="K37" s="16">
         <v>0</v>
       </c>
       <c r="L37" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M37" s="42">
+      <c r="M37" s="38">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="83"/>
-      <c r="B38" s="25" t="s">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="77"/>
+      <c r="B38" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="18">
+      <c r="C38" s="16">
         <v>13</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E38" s="42">
+      <c r="E38" s="38">
         <v>20</v>
       </c>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="86"/>
-      <c r="J38" s="22" t="s">
+      <c r="I38" s="80"/>
+      <c r="J38" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K38" s="18">
+      <c r="K38" s="16">
         <v>1</v>
       </c>
-      <c r="L38" s="19" t="s">
+      <c r="L38" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="M38" s="42">
+      <c r="M38" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="83"/>
-      <c r="B39" s="24" t="s">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="77"/>
+      <c r="B39" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="18">
-        <v>18</v>
+      <c r="C39" s="16">
+        <v>17</v>
       </c>
       <c r="D39" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E39" s="42">
+      <c r="E39" s="38">
         <v>16</v>
       </c>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="86"/>
-      <c r="J39" s="23" t="s">
+      <c r="I39" s="80"/>
+      <c r="J39" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="K39" s="18">
+      <c r="K39" s="16">
         <v>2</v>
       </c>
       <c r="L39" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="M39" s="42">
+      <c r="M39" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="84"/>
-      <c r="B40" s="45" t="s">
+    <row r="40" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="78"/>
+      <c r="B40" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="33">
+      <c r="C40" s="29">
         <v>14</v>
       </c>
-      <c r="D40" s="34" t="s">
+      <c r="D40" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="E40" s="43">
+      <c r="E40" s="39">
+        <v>16</v>
+      </c>
+      <c r="I40" s="81"/>
+      <c r="J40" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="29">
+        <v>2</v>
+      </c>
+      <c r="L40" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="M40" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="76">
+        <v>2025</v>
+      </c>
+      <c r="B41" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="26">
+        <v>13</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="37"/>
+      <c r="I41" s="76">
+        <v>2025</v>
+      </c>
+      <c r="J41" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="K41" s="26">
+        <v>1</v>
+      </c>
+      <c r="L41" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="M41" s="37"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="77"/>
+      <c r="B42" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="16">
+        <v>20</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="38"/>
+      <c r="I42" s="77"/>
+      <c r="J42" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K42" s="16">
+        <v>1</v>
+      </c>
+      <c r="L42" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M42" s="38"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="77"/>
+      <c r="B43" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="16">
+        <v>16</v>
+      </c>
+      <c r="D43" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="87"/>
-      <c r="J40" s="32" t="s">
+      <c r="E43" s="38"/>
+      <c r="I43" s="77"/>
+      <c r="J43" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="K43" s="16">
+        <v>1</v>
+      </c>
+      <c r="L43" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="M43" s="38"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="77"/>
+      <c r="B44" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="16">
+        <v>17</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="38"/>
+      <c r="I44" s="77"/>
+      <c r="J44" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="K44" s="16">
+        <v>2</v>
+      </c>
+      <c r="L44" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="M44" s="38"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="77"/>
+      <c r="B45" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="16">
+        <v>17</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="38"/>
+      <c r="I45" s="77"/>
+      <c r="J45" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="K45" s="16">
+        <v>4</v>
+      </c>
+      <c r="L45" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M45" s="38"/>
+    </row>
+    <row r="46" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="78"/>
+      <c r="B46" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="K40" s="33">
-        <v>2</v>
-      </c>
-      <c r="L40" s="34" t="s">
+      <c r="C46" s="29"/>
+      <c r="D46" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="M40" s="43">
+      <c r="E46" s="39"/>
+      <c r="I46" s="78"/>
+      <c r="J46" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="K46" s="29"/>
+      <c r="L46" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="M46" s="39"/>
+    </row>
+    <row r="47" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="1:13" ht="31.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="47" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" ht="15">
-      <c r="A42" s="51" t="s">
+      <c r="B48" s="64" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="70" t="s">
-        <v>18</v>
-      </c>
-      <c r="I42" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="J42" s="69" t="s">
+      <c r="J48" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="M42" s="28"/>
-    </row>
-    <row r="43" spans="1:13" ht="21" customHeight="1">
-      <c r="A43" s="59">
+    </row>
+    <row r="49" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="103">
         <v>2019</v>
       </c>
-      <c r="B43" s="53">
+      <c r="B49" s="97">
         <v>143</v>
       </c>
-      <c r="I43" s="65">
+      <c r="I49" s="59">
         <v>2019</v>
       </c>
-      <c r="J43" s="53">
+      <c r="J49" s="49">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="15">
-      <c r="A44" s="60">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="104">
         <v>2020</v>
       </c>
-      <c r="B44" s="54">
+      <c r="B50" s="44">
         <v>128</v>
       </c>
-      <c r="I44" s="66">
+      <c r="I50" s="60">
         <v>2020</v>
       </c>
-      <c r="J44" s="54">
+      <c r="J50" s="50">
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="15">
-      <c r="A45" s="61">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="105">
         <v>2021</v>
       </c>
-      <c r="B45" s="55">
-        <v>141</v>
-      </c>
-      <c r="F45" s="28"/>
-      <c r="I45" s="67">
+      <c r="B51" s="98">
+        <v>139</v>
+      </c>
+      <c r="I51" s="61">
         <v>2021</v>
       </c>
-      <c r="J45" s="55">
+      <c r="J51" s="51">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="15">
-      <c r="A46" s="62">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="106">
         <v>2022</v>
       </c>
-      <c r="B46" s="56">
+      <c r="B52" s="99">
         <v>169</v>
       </c>
-      <c r="F46" s="28"/>
-      <c r="I46" s="68">
+      <c r="I52" s="62">
         <v>2022</v>
       </c>
-      <c r="J46" s="56">
+      <c r="J52" s="52">
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="15">
-      <c r="A47" s="63">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="107">
         <v>2023</v>
       </c>
-      <c r="B47" s="57">
-        <v>145</v>
-      </c>
-      <c r="F47" s="28"/>
-      <c r="I47" s="68">
+      <c r="B53" s="100">
+        <v>144</v>
+      </c>
+      <c r="I53" s="62">
         <v>2023</v>
       </c>
-      <c r="J47" s="56">
+      <c r="J53" s="52">
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="15">
-      <c r="A48" s="63">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="105">
         <v>2024</v>
       </c>
-      <c r="B48" s="55">
-        <v>182</v>
-      </c>
-      <c r="F48" s="28"/>
-      <c r="I48" s="68">
+      <c r="B54" s="101">
+        <v>186</v>
+      </c>
+      <c r="I54" s="62">
         <v>2024</v>
       </c>
-      <c r="J48" s="56">
+      <c r="J54" s="52">
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
-      <c r="A49" s="64" t="s">
+    <row r="55" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="105">
+        <v>2025</v>
+      </c>
+      <c r="B55" s="101">
+        <v>83</v>
+      </c>
+      <c r="I55" s="109">
+        <v>2025</v>
+      </c>
+      <c r="J55" s="53">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="B49" s="58">
-        <v>908</v>
-      </c>
-      <c r="F49" s="28"/>
-      <c r="I49" s="64" t="s">
+      <c r="B56" s="102">
+        <f>SUM(Table1[Total con querella])</f>
+        <v>992</v>
+      </c>
+      <c r="I56" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="J49" s="58">
-        <v>220</v>
+      <c r="J56" s="111">
+        <f>SUM(J49:J55)</f>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="17">
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="I41:I46"/>
     <mergeCell ref="A35:A40"/>
     <mergeCell ref="I35:I40"/>
     <mergeCell ref="A1:M1"/>
@@ -3131,88 +3491,101 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="29.25" thickBot="1">
-      <c r="A1" s="80" t="s">
+    <row r="1" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="73" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1">
-      <c r="A2" s="59">
+    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="54">
         <v>2019</v>
       </c>
-      <c r="B2" s="53">
+      <c r="B2" s="49">
         <v>143</v>
       </c>
-      <c r="C2" s="53">
+      <c r="C2" s="49">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15">
-      <c r="A3" s="60">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="55">
         <v>2020</v>
       </c>
-      <c r="B3" s="54">
+      <c r="B3" s="50">
         <v>128</v>
       </c>
-      <c r="C3" s="54">
+      <c r="C3" s="50">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15">
-      <c r="A4" s="61">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="56">
         <v>2021</v>
       </c>
-      <c r="B4" s="55">
-        <v>141</v>
-      </c>
-      <c r="C4" s="55">
+      <c r="B4" s="51">
+        <v>139</v>
+      </c>
+      <c r="C4" s="51">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15">
-      <c r="A5" s="62">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="57">
         <v>2022</v>
       </c>
-      <c r="B5" s="56">
+      <c r="B5" s="52">
         <v>169</v>
       </c>
-      <c r="C5" s="56">
+      <c r="C5" s="52">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15">
-      <c r="A6" s="63">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="58">
         <v>2023</v>
       </c>
-      <c r="B6" s="57">
-        <v>145</v>
-      </c>
-      <c r="C6" s="56">
+      <c r="B6" s="53">
+        <v>144</v>
+      </c>
+      <c r="C6" s="52">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15">
-      <c r="A7" s="62">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="57">
         <v>2024</v>
       </c>
-      <c r="B7" s="81">
-        <v>182</v>
-      </c>
-      <c r="C7" s="56">
+      <c r="B7" s="75">
+        <v>186</v>
+      </c>
+      <c r="C7" s="52">
         <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="57">
+        <v>2025</v>
+      </c>
+      <c r="B8" s="75">
+        <v>83</v>
+      </c>
+      <c r="C8" s="52">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -3221,33 +3594,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="80" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="80" t="s">
+      <c r="D1" s="74" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -3261,7 +3636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -3275,7 +3650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -3289,7 +3664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -3303,7 +3678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2023</v>
       </c>
@@ -3317,18 +3692,137 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2024</v>
       </c>
       <c r="B7">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C7">
         <v>88</v>
       </c>
       <c r="D7">
         <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2025</v>
+      </c>
+      <c r="B8">
+        <v>44</v>
+      </c>
+      <c r="C8">
+        <v>39</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5F89AC2-02D9-4754-B035-F9ADADF99A64}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.109375" customWidth="1"/>
+    <col min="4" max="4" width="32.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="112" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="112" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="112" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="112" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2021</v>
+      </c>
+      <c r="B2">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>330</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2022</v>
+      </c>
+      <c r="B3">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>583</v>
+      </c>
+      <c r="D3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2023</v>
+      </c>
+      <c r="B4">
+        <v>119</v>
+      </c>
+      <c r="C4">
+        <v>267</v>
+      </c>
+      <c r="D4">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2024</v>
+      </c>
+      <c r="B5">
+        <v>130</v>
+      </c>
+      <c r="C5">
+        <v>178</v>
+      </c>
+      <c r="D5">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2025</v>
+      </c>
+      <c r="B6">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>